<commit_message>
Nifty 50 Golden Cross Tracker - added readme.md
</commit_message>
<xml_diff>
--- a/code/output/nifty50_golden_cross.xlsx
+++ b/code/output/nifty50_golden_cross.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,21 +479,21 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>TECHM.NS</t>
+          <t>ASIANPAINT.NS</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Ticker
-TECHM.NS    1486.699951
+ASIANPAINT.NS    2528.699951
 Name: 2025-08-14 00:00:00, dtype: float64</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1571.684790039063</v>
+        <v>2371.580483398438</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>1571.120545043945</v>
+        <v>2352.398364257812</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>45881</v>
@@ -505,21 +505,21 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>ASIANPAINT.NS</t>
+          <t>TECHM.NS</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
           <t>Ticker
-ASIANPAINT.NS    2528.699951
+TECHM.NS    1486.699951
 Name: 2025-08-14 00:00:00, dtype: float64</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>2371.580483398438</v>
+        <v>1571.684790039063</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>2352.398364257812</v>
+        <v>1571.120545043945</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>45881</v>
@@ -661,104 +661,130 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DRREDDY.NS</t>
+          <t>JIOFIN.NS</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Ticker
-DRREDDY.NS    1260.400024
+JIOFIN.NS    327.399994
 Name: 2025-08-14 00:00:00, dtype: float64</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1277.604030761719</v>
+        <v>315.1475115966797</v>
       </c>
       <c r="D9" t="n">
-        <v>1231.427052612305</v>
+        <v>281.9188722229004</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>45838</v>
+        <v>45842</v>
       </c>
       <c r="F9" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>LT.NS</t>
+          <t>DRREDDY.NS</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>Ticker
-LT.NS    3677.0
+DRREDDY.NS    1260.400024
 Name: 2025-08-14 00:00:00, dtype: float64</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3593.316005859375</v>
+        <v>1277.604030761719</v>
       </c>
       <c r="D10" t="n">
-        <v>3485.814195556641</v>
+        <v>1231.427052612305</v>
       </c>
       <c r="E10" s="4" t="n">
-        <v>45832</v>
+        <v>45838</v>
       </c>
       <c r="F10" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>M&amp;M.NS</t>
+          <t>LT.NS</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>Ticker
-M&amp;M.NS    3265.399902
+LT.NS    3677.0
 Name: 2025-08-14 00:00:00, dtype: float64</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3155.26541015625</v>
+        <v>3593.316005859375</v>
       </c>
       <c r="D11" t="n">
-        <v>2955.768426513672</v>
+        <v>3485.814195556641</v>
       </c>
       <c r="E11" s="4" t="n">
-        <v>45821</v>
+        <v>45832</v>
       </c>
       <c r="F11" t="n">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>M&amp;M.NS</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Ticker
+M&amp;M.NS    3265.399902
+Name: 2025-08-14 00:00:00, dtype: float64</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>3155.26541015625</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2955.768426513672</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>45821</v>
+      </c>
+      <c r="F12" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>TITAN.NS</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>Ticker
 TITAN.NS    3489.399902
 Name: 2025-08-14 00:00:00, dtype: float64</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C13" t="n">
         <v>3483.054565429688</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D13" t="n">
         <v>3351.148258056641</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="E13" s="4" t="n">
         <v>45818</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F13" t="n">
         <v>68</v>
       </c>
     </row>

</xml_diff>